<commit_message>
Success for Create Looping Request
</commit_message>
<xml_diff>
--- a/YouTube Channel KOMPASTV/Results of Data Exports from DataFrame/Export Comments Data from 2nd Video Debate.xlsx
+++ b/YouTube Channel KOMPASTV/Results of Data Exports from DataFrame/Export Comments Data from 2nd Video Debate.xlsx
@@ -55,12 +55,12 @@
     <t>UgzXUiEcKGGoUX0nDeh4AaABAg</t>
   </si>
   <si>
+    <t>UgyBOQDTIbXXmH8m1Vx4AaABAg</t>
+  </si>
+  <si>
     <t>Ugypp9rnOjLTrXH5Tb14AaABAg</t>
   </si>
   <si>
-    <t>UgyBOQDTIbXXmH8m1Vx4AaABAg</t>
-  </si>
-  <si>
     <t>Ugzjx9OYz33QH4J6IlF4AaABAg</t>
   </si>
   <si>
@@ -1555,12 +1555,12 @@
     <t>@ariessusanti-ep2or</t>
   </si>
   <si>
+    <t>@melisa8319</t>
+  </si>
+  <si>
     <t>@anisatulainiyah1001</t>
   </si>
   <si>
-    <t>@melisa8319</t>
-  </si>
-  <si>
     <t>@wargaproxima7105</t>
   </si>
   <si>
@@ -2758,12 +2758,12 @@
     <t>Gibran ternyata gak spt yg disangka sangka, pernyataannya lugas, tegas, jelas dan cerdas ..</t>
   </si>
   <si>
+    <t>Sempet skeptis sama gibran karna bantuan paman tapi setelah nonton ini membuka mata banget publik speaking muda keren banget</t>
+  </si>
+  <si>
     <t>Serius merinding dengar gibran jawab. Secerdass itu. Semoga bisaa memimpin indonesia ke depannya.</t>
   </si>
   <si>
-    <t>Sempet skeptis sama gibran karna bantuan paman tapi setelah nonton ini membuka mata banget publik speaking muda keren banget</t>
-  </si>
-  <si>
     <t>Anak muda memang berfikirnya praktis, tidak muter-muter dan bertele-tele. Sudah saatnya kita memiliki pemimpin yang muda dan melek dengan jaman ini</t>
   </si>
   <si>
@@ -4249,10 +4249,10 @@
     <t>http://www.youtube.com/@ariessusanti-ep2or</t>
   </si>
   <si>
+    <t>http://www.youtube.com/@melisa8319</t>
+  </si>
+  <si>
     <t>http://www.youtube.com/@anisatulainiyah1001</t>
-  </si>
-  <si>
-    <t>http://www.youtube.com/@melisa8319</t>
   </si>
   <si>
     <t>http://www.youtube.com/@wargaproxima7105</t>
@@ -5908,19 +5908,19 @@
         <v>914</v>
       </c>
       <c r="F3">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G3">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>1411</v>
       </c>
       <c r="I3" s="3">
-        <v>45291.07915509259</v>
+        <v>45290.62524305555</v>
       </c>
       <c r="J3" s="3">
-        <v>45291.07915509259</v>
+        <v>45290.62524305555</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -5943,16 +5943,16 @@
         <v>84</v>
       </c>
       <c r="G4">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>1412</v>
       </c>
       <c r="I4" s="3">
-        <v>45290.62524305555</v>
+        <v>45291.07915509259</v>
       </c>
       <c r="J4" s="3">
-        <v>45290.62524305555</v>
+        <v>45291.07915509259</v>
       </c>
     </row>
     <row r="5" spans="1:10">

</xml_diff>